<commit_message>
added Catalan and Czech
</commit_message>
<xml_diff>
--- a/Localization/PopGuide_Translations_V7.xlsx
+++ b/Localization/PopGuide_Translations_V7.xlsx
@@ -140,7 +140,7 @@
     <t xml:space="preserve">zh</t>
   </si>
   <si>
-    <t xml:space="preserve">cz</t>
+    <t xml:space="preserve">cs</t>
   </si>
   <si>
     <t xml:space="preserve">ca</t>
@@ -173,6 +173,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">한국어 </t>
     </r>
@@ -1494,6 +1495,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">주의</t>
     </r>
@@ -1549,6 +1551,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">실패</t>
     </r>
@@ -1607,6 +1610,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">경로를 찾던 중 오류가 발생했습니다</t>
     </r>
@@ -1704,6 +1708,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">現在地を計算するには位置情報サービスが必要です。</t>
     </r>
@@ -1721,6 +1726,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">アプリの設定から有効にして下さい。</t>
     </r>
@@ -1731,6 +1737,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">현재 위치를 찾으려면 위치 서비스가 필요합니다</t>
     </r>
@@ -1748,6 +1755,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">앱 설정에서 사용하도록 설정하십시오</t>
     </r>
@@ -1776,6 +1784,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">计算当前位置所需地点服务功能</t>
     </r>
@@ -1793,6 +1802,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">请从应用程序的设置中启动</t>
     </r>
@@ -1830,6 +1840,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">다른 계정으로 전환하고 있습니다</t>
     </r>
@@ -1888,6 +1899,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">네트워크 오류</t>
     </r>
@@ -1943,6 +1955,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">インターネットの接続が見つかりません。</t>
     </r>
@@ -1960,6 +1973,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">再度お試しください。</t>
     </r>
@@ -1970,6 +1984,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">인터넷 연결을 찾을 수 없습니다</t>
     </r>
@@ -1987,6 +2002,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">나중에 다시 시도하십시오</t>
     </r>
@@ -2015,6 +2031,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">未找到网络连接。</t>
     </r>
@@ -2032,6 +2049,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">请稍后再试</t>
     </r>
@@ -2066,6 +2084,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">携帯電話ネットワークで大量のデータをダウンロードすることはお勧めしません。 パッケージをダウンロードするには</t>
     </r>
@@ -2083,6 +2102,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ネットワークに接続して下さい。</t>
     </r>
@@ -2093,6 +2113,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">모바일 네트워크로 대용량 데이터를 다운로드하는 것은 권장하지 않습니다</t>
     </r>
@@ -2110,6 +2131,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">패키지 다운로드를 위해 </t>
     </r>
@@ -2127,6 +2149,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">네트워크에 연결하십시오</t>
     </r>
@@ -2155,6 +2178,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">我们不建议在蜂窝网络上下载大量数据。请连接</t>
     </r>
@@ -2172,6 +2196,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">网络以下载套装软件</t>
     </r>
@@ -2209,6 +2234,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">계속 사용하려면 앱을 업데이트 해야합니다</t>
     </r>
@@ -2306,6 +2332,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">あなたの現在地は圏外です</t>
     </r>
@@ -2323,6 +2350,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ルート計算とナビゲーションはできません。</t>
     </r>
@@ -2333,6 +2361,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">현재 위치가 도시 제한을 벗어났습니다</t>
     </r>
@@ -2350,6 +2379,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">경로 계산 및 탐색이 불가능합니다</t>
     </r>
@@ -2378,6 +2408,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">您当前的位置超出城区范围</t>
     </r>
@@ -2395,6 +2426,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">路线计算及导航无法使用</t>
     </r>
@@ -2474,6 +2506,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">사용자 이름과 암호를 입력하십시오</t>
     </r>
@@ -2575,6 +2608,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">사용자 이름과 암호를 확인한 후 다시 시도하십시오</t>
     </r>
@@ -2630,6 +2664,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ダウンロード中にエラーが生じました。</t>
     </r>
@@ -2647,6 +2682,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">もう一度やり直して下さい。</t>
     </r>
@@ -2657,6 +2693,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">패키지 다운로드 중 오류가 발생했습니다</t>
     </r>
@@ -2674,6 +2711,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">다시 시도하십시오</t>
     </r>
@@ -2702,6 +2740,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">下载旅游包时出现错误</t>
     </r>
@@ -2719,6 +2758,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">请重试</t>
     </r>
@@ -2837,6 +2877,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">データの同期中にエラーが発生しました！</t>
     </r>
@@ -2854,6 +2895,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">もう一度お試しください。</t>
     </r>
@@ -2864,6 +2906,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">데이터 동기화 중 오류가 발생했습니다</t>
     </r>
@@ -2881,6 +2924,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">나중에 다시 시도하십시오</t>
     </r>
@@ -2935,6 +2979,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">同步数据时发生了一些错误！</t>
     </r>
@@ -2952,6 +2997,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">请稍后再试</t>
     </r>
@@ -3031,6 +3077,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">작업 수행 중 오류가 발생했습니다</t>
     </r>
@@ -3095,6 +3142,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">良い旅を！</t>
     </r>
@@ -3105,6 +3153,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">좋은 여행이 되십시오</t>
     </r>
@@ -3142,6 +3191,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">旅途愉快！</t>
     </r>
@@ -3176,6 +3226,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">あなたが設定したツアーガイドは</t>
     </r>
@@ -3193,6 +3244,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">からご利用頂けます。</t>
     </r>
@@ -3203,6 +3255,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">당신의 </t>
     </r>
@@ -3220,6 +3273,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">맞춤 여행 가이드를 지금 검색 할 수 있습니다</t>
     </r>
@@ -3248,6 +3302,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">％</t>
     </r>
@@ -3265,6 +3320,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">为您的私人订制已就绪！</t>
     </r>
@@ -3341,6 +3397,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">オーディオガイドの更新が可能です。</t>
     </r>
@@ -3358,6 +3415,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">今すぐダウンロードしますか？</t>
     </r>
@@ -3368,6 +3426,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">오디오 가이드의 업데이트를 다운로드 할 수 있습니다</t>
     </r>
@@ -3385,6 +3444,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">지금 다운로드하시겠습니까</t>
     </r>
@@ -3413,6 +3473,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">此语音导览的更新可以下载。</t>
     </r>
@@ -3430,6 +3491,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">是否要立即下载？</t>
     </r>
@@ -3467,6 +3529,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">삭제하시겠습니까</t>
     </r>
@@ -3522,6 +3585,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">このツァーの内容を削除しますか？</t>
     </r>
@@ -3539,6 +3603,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ツアーのエントリは引き続きこのリストに表示され、将来コンテンツを再ダウンロードすることができます。</t>
     </r>
@@ -3549,6 +3614,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">이 여행을 삭제 하시겠습니까</t>
     </r>
@@ -3566,6 +3632,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">이 여행은 다시 다운로드 할 수 있습니다</t>
     </r>
@@ -3620,6 +3687,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">您确定要删除此次行程的内容吗？</t>
     </r>
@@ -3637,6 +3705,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">行程”的条目将继续显示在此列表中，以便您将来可以重新下载该内容。</t>
     </r>
@@ -3672,6 +3741,7 @@
         <color rgb="FF333333"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">続行するには、</t>
     </r>
@@ -3691,6 +3761,7 @@
         <color rgb="FF333333"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">のロケーションサービスをオンにして、地図がローミング料金を発生させずにオフラインで機能するようにします。</t>
     </r>
@@ -3701,6 +3772,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">계속하려면 </t>
     </r>
@@ -3718,6 +3790,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">가 위치 서비스를 사용하도록 설정해 로밍 요금을 부과 없이 지도를 오프라인으로 작동할 수 있게 합니다</t>
     </r>
@@ -3746,6 +3819,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">为了继续，请您允许设备打开</t>
     </r>
@@ -3763,6 +3837,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">的位置服务，以便使地图可离线工作，从而不会产生漫游费用</t>
     </r>
@@ -3808,6 +3883,7 @@
         <color rgb="FF333333"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">コードスキャナにはカメラ権限が必要です。 アプリの設定から有効にしてください。</t>
     </r>
@@ -3827,6 +3903,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">코드 스캐너에 카메라가 필요합니다</t>
     </r>
@@ -3844,6 +3921,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">앱 설정에서 활성화하십시오</t>
     </r>
@@ -3899,6 +3977,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">로그아웃 하시겠습니까</t>
     </r>
@@ -3955,6 +4034,7 @@
         <color rgb="FF333333"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">このアカウントから本当にログアウトしますか？</t>
     </r>
@@ -3974,6 +4054,7 @@
         <color rgb="FF333333"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">関連するすべてのオーディオガイドも削除されます！</t>
     </r>
@@ -3984,6 +4065,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">이 계정에서 정말 로그아웃하시겠습니까</t>
     </r>
@@ -4001,6 +4083,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">관련된 오디오 가이드도 모두 제거됩니다</t>
     </r>
@@ -4029,6 +4112,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">您真的要从此账号退出吗？</t>
     </r>
@@ -4046,6 +4130,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">所有相关的语音导览也将被清除</t>
     </r>
@@ -4089,6 +4174,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">が有効になっていません。</t>
     </r>
@@ -4108,6 +4194,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">해제</t>
     </r>
@@ -4136,6 +4223,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">无法启用</t>
     </r>
@@ -4179,6 +4267,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">を有効にしてもう一度お試し下さい。</t>
     </r>
@@ -4198,6 +4287,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">를 사용하도록 설정하고 다시 시도하십시오</t>
     </r>
@@ -4226,6 +4316,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">请启用</t>
     </r>
@@ -4243,6 +4334,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">并重试</t>
     </r>
@@ -4441,6 +4533,7 @@
         <color rgb="FF000000"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">コードをスキャンするにはここをクリックしてください</t>
     </r>
@@ -4460,6 +4553,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">코드를 스캔하려면 여기를 누르십시오</t>
     </r>
@@ -4488,6 +4582,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">点击此处扫描</t>
     </r>
@@ -4505,6 +4600,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">码</t>
     </r>
@@ -5064,6 +5160,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">包含</t>
     </r>
@@ -5081,6 +5178,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">未包含</t>
     </r>
@@ -5505,6 +5603,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">感谢订购！</t>
     </r>
@@ -5522,6 +5621,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">将收到邮件确认函，包含订单详情</t>
     </r>
@@ -5760,6 +5860,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">总人数应该在</t>
     </r>
@@ -5777,6 +5878,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">到</t>
     </r>
@@ -5794,6 +5896,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">之间</t>
     </r>
@@ -6068,6 +6171,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">在支付过程中出现错误</t>
     </r>
@@ -6085,6 +6189,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">请查看信用卡信息后重试</t>
     </r>
@@ -6191,6 +6296,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">进入商城服务，需连接网络</t>
     </r>
@@ -6208,6 +6314,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">请查看您的网络连接</t>
     </r>
@@ -6225,6 +6332,7 @@
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">点击以下按键重试</t>
     </r>
@@ -6349,6 +6457,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">继续，同意我们的 </t>
     </r>
@@ -6366,6 +6475,7 @@
         <sz val="11"/>
         <rFont val="Microsoft YaHei"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">条款及细则</t>
     </r>
@@ -6911,6 +7021,7 @@
       <sz val="11"/>
       <name val="Microsoft YaHei"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -6929,6 +7040,7 @@
       <sz val="10"/>
       <name val="Microsoft YaHei"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -6942,6 +7054,7 @@
       <color rgb="FF000000"/>
       <name val="Microsoft YaHei"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -6973,6 +7086,7 @@
       <sz val="11"/>
       <name val="Microsoft YaHei"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -6985,6 +7099,7 @@
       <color rgb="FF333333"/>
       <name val="Microsoft YaHei"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -7520,11 +7635,11 @@
   <dimension ref="A1:AA140"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B134" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A134" activeCellId="0" sqref="A134"/>
-      <selection pane="bottomRight" activeCell="A140" activeCellId="0" sqref="A140"/>
+      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="X2" activeCellId="0" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7535,7 +7650,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="28" style="0" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>